<commit_message>
fix: Começo leitura planilha modelo PDO
</commit_message>
<xml_diff>
--- a/Modelo_PDO.xlsx
+++ b/Modelo_PDO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70ac05f72bfee68d/Documentos/GUAIBA/ERGTools/bin/Debug/net7.0-windows/Modelos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rogerio.piccoli\OneDrive\Documentos\GUAIBA\Python\ERG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_532C1937D002C57011ABAAF7D521FB25254987A4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69634D87-8803-4CAA-A7C6-6DC32DE29C54}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87B8B8C-8DA1-441F-818B-24712D848924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conferência" sheetId="10" r:id="rId1"/>
@@ -2214,100 +2214,152 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>23813</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>11907</xdr:rowOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>892968</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1285875</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>673659</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>97471</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1" descr="image">
+        <xdr:cNvPr id="3" name="Imagem 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A728A4A-49B4-E20D-FAE2-95CC5948B3E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="23813" y="11907"/>
-          <a:ext cx="2000249" cy="1273968"/>
+          <a:off x="46148625" y="5441156"/>
+          <a:ext cx="1876190" cy="1276190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>898551</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:rowOff>23813</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1352298</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>892734</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1166813</xdr:rowOff>
+      <xdr:rowOff>1300003</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Imagem 1" descr="Logo Metroplan.jpg">
+        <xdr:cNvPr id="5" name="Imagem 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98B27B09-0BFD-04BC-92E2-320E91CD10AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect t="20869" b="19977"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="8732864" y="95251"/>
-          <a:ext cx="4001809" cy="1071562"/>
+          <a:off x="28575" y="23813"/>
+          <a:ext cx="1873809" cy="1276190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1219199</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1321896</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1139016</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{614A3F3C-7796-4CB2-7202-2757A1F54ECA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8372474" y="161191"/>
+          <a:ext cx="3645997" cy="977825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2699,7 +2751,7 @@
   </sheetPr>
   <dimension ref="A1:AK50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -5753,8 +5805,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:AT24"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AO22" sqref="AO22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: Incluída leitura e merge das viagens previstas Met
</commit_message>
<xml_diff>
--- a/Modelo_PDO.xlsx
+++ b/Modelo_PDO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rogerio.piccoli\OneDrive\Documentos\GUAIBA\Python\ERG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70ac05f72bfee68d/Documentos/GUAIBA/Python/ERG/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD637E1-B1AE-4745-9C24-AB7A4DFFDC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -1327,6 +1327,10 @@
     <xf numFmtId="165" fontId="12" fillId="9" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="12" fillId="9" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="12" fillId="9" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="9" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="9" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="9" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="9" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1336,6 +1340,36 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1343,6 +1377,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1377,57 +1432,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1458,20 +1462,11 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="9" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="9" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="9" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="9" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1551,91 +1546,6 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2480,43 +2390,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1382" displayName="Tabela1382" ref="A10:F11" insertRow="1" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1382" displayName="Tabela1382" ref="A10:F11" insertRow="1" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A10:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DIAS ÚTEIS" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SABADOS " dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DIAS ÚTEIS2" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SABADOS 2" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DIAS ÚTEIS" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SABADOS " dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DIAS ÚTEIS2" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SABADOS 2" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela13493" displayName="Tabela13493" ref="A14:F15" insertRow="1" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela13493" displayName="Tabela13493" ref="A14:F15" insertRow="1" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A14:F15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DIAS ÚTEIS" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SABADOS " dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DIAS ÚTEIS2" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="SABADOS 2" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DIAS ÚTEIS" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SABADOS " dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DIAS ÚTEIS2" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="SABADOS 2" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela94" displayName="Tabela94" ref="A4:D7" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela94" displayName="Tabela94" ref="A4:D7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="A4:D7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="####" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Total de Viagens Oficiais " dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Total de Viagens Extras" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Km's Totais" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="####" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Total de Viagens Oficiais " dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Total de Viagens Extras" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Km's Totais" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2814,7 +2724,7 @@
   </sheetPr>
   <dimension ref="A1:AK50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AO27" sqref="AO27"/>
     </sheetView>
   </sheetViews>
@@ -2824,98 +2734,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="61" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="61" t="s">
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="62"/>
-      <c r="AK1" s="63"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="67"/>
     </row>
     <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="61" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="61" t="s">
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="61" t="s">
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="63"/>
-      <c r="Z2" s="61" t="s">
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="61" t="s">
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="62"/>
-      <c r="AJ2" s="62"/>
-      <c r="AK2" s="63"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="66"/>
+      <c r="AJ2" s="66"/>
+      <c r="AK2" s="67"/>
     </row>
     <row r="3" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
@@ -3039,7 +2949,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="49"/>
-      <c r="F4" s="106"/>
+      <c r="F4" s="61"/>
       <c r="G4" s="50">
         <f>D4+E4-F4</f>
         <v>0</v>
@@ -3051,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="49"/>
-      <c r="L4" s="106"/>
+      <c r="L4" s="61"/>
       <c r="M4" s="50">
         <f>J4+K4-L4</f>
         <v>0</v>
@@ -3063,7 +2973,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="49"/>
-      <c r="R4" s="106"/>
+      <c r="R4" s="61"/>
       <c r="S4" s="50">
         <f>P4+Q4-R4</f>
         <v>0</v>
@@ -3075,7 +2985,7 @@
         <v>0</v>
       </c>
       <c r="W4" s="49"/>
-      <c r="X4" s="106"/>
+      <c r="X4" s="61"/>
       <c r="Y4" s="50">
         <f>V4+W4-X4</f>
         <v>0</v>
@@ -3087,7 +2997,7 @@
         <v>0</v>
       </c>
       <c r="AC4" s="49"/>
-      <c r="AD4" s="106"/>
+      <c r="AD4" s="61"/>
       <c r="AE4" s="50">
         <f>AB4+AC4-AD4</f>
         <v>0</v>
@@ -3099,7 +3009,7 @@
         <v>0</v>
       </c>
       <c r="AI4" s="49"/>
-      <c r="AJ4" s="106"/>
+      <c r="AJ4" s="61"/>
       <c r="AK4" s="50">
         <f>AH4+AI4-AJ4</f>
         <v>0</v>
@@ -3114,7 +3024,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="53"/>
-      <c r="F5" s="107"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="50">
         <f t="shared" ref="G5:G49" si="1">D5+E5-F5</f>
         <v>0</v>
@@ -3126,7 +3036,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="53"/>
-      <c r="L5" s="107"/>
+      <c r="L5" s="62"/>
       <c r="M5" s="50">
         <f t="shared" ref="M5:M49" si="3">J5+K5-L5</f>
         <v>0</v>
@@ -3138,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="53"/>
-      <c r="R5" s="107"/>
+      <c r="R5" s="62"/>
       <c r="S5" s="50">
         <f t="shared" ref="S5:S49" si="5">P5+Q5-R5</f>
         <v>0</v>
@@ -3150,7 +3060,7 @@
         <v>0</v>
       </c>
       <c r="W5" s="53"/>
-      <c r="X5" s="107"/>
+      <c r="X5" s="62"/>
       <c r="Y5" s="50">
         <f t="shared" ref="Y5:Y49" si="7">V5+W5-X5</f>
         <v>0</v>
@@ -3162,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="AC5" s="53"/>
-      <c r="AD5" s="107"/>
+      <c r="AD5" s="62"/>
       <c r="AE5" s="50">
         <f t="shared" ref="AE5:AE49" si="9">AB5+AC5-AD5</f>
         <v>0</v>
@@ -3174,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="AI5" s="53"/>
-      <c r="AJ5" s="107"/>
+      <c r="AJ5" s="62"/>
       <c r="AK5" s="50">
         <f t="shared" ref="AK5:AK49" si="11">AH5+AI5-AJ5</f>
         <v>0</v>
@@ -3189,7 +3099,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="53"/>
-      <c r="F6" s="107"/>
+      <c r="F6" s="62"/>
       <c r="G6" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3201,7 +3111,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="53"/>
-      <c r="L6" s="107"/>
+      <c r="L6" s="62"/>
       <c r="M6" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3213,7 +3123,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="53"/>
-      <c r="R6" s="107"/>
+      <c r="R6" s="62"/>
       <c r="S6" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3225,7 +3135,7 @@
         <v>0</v>
       </c>
       <c r="W6" s="53"/>
-      <c r="X6" s="107"/>
+      <c r="X6" s="62"/>
       <c r="Y6" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3237,7 +3147,7 @@
         <v>0</v>
       </c>
       <c r="AC6" s="53"/>
-      <c r="AD6" s="107"/>
+      <c r="AD6" s="62"/>
       <c r="AE6" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3249,7 +3159,7 @@
         <v>0</v>
       </c>
       <c r="AI6" s="53"/>
-      <c r="AJ6" s="107"/>
+      <c r="AJ6" s="62"/>
       <c r="AK6" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3264,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="53"/>
-      <c r="F7" s="107"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3276,7 +3186,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="53"/>
-      <c r="L7" s="107"/>
+      <c r="L7" s="62"/>
       <c r="M7" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3288,7 +3198,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="53"/>
-      <c r="R7" s="107"/>
+      <c r="R7" s="62"/>
       <c r="S7" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3300,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="W7" s="53"/>
-      <c r="X7" s="107"/>
+      <c r="X7" s="62"/>
       <c r="Y7" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3312,7 +3222,7 @@
         <v>0</v>
       </c>
       <c r="AC7" s="53"/>
-      <c r="AD7" s="107"/>
+      <c r="AD7" s="62"/>
       <c r="AE7" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3324,7 +3234,7 @@
         <v>0</v>
       </c>
       <c r="AI7" s="53"/>
-      <c r="AJ7" s="107"/>
+      <c r="AJ7" s="62"/>
       <c r="AK7" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3339,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="53"/>
-      <c r="F8" s="107"/>
+      <c r="F8" s="62"/>
       <c r="G8" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3351,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="53"/>
-      <c r="L8" s="107"/>
+      <c r="L8" s="62"/>
       <c r="M8" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3363,7 +3273,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="53"/>
-      <c r="R8" s="107"/>
+      <c r="R8" s="62"/>
       <c r="S8" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3375,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="W8" s="53"/>
-      <c r="X8" s="107"/>
+      <c r="X8" s="62"/>
       <c r="Y8" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3387,7 +3297,7 @@
         <v>0</v>
       </c>
       <c r="AC8" s="53"/>
-      <c r="AD8" s="107"/>
+      <c r="AD8" s="62"/>
       <c r="AE8" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3399,7 +3309,7 @@
         <v>0</v>
       </c>
       <c r="AI8" s="53"/>
-      <c r="AJ8" s="107"/>
+      <c r="AJ8" s="62"/>
       <c r="AK8" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3414,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="53"/>
-      <c r="F9" s="107"/>
+      <c r="F9" s="62"/>
       <c r="G9" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3426,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="53"/>
-      <c r="L9" s="107"/>
+      <c r="L9" s="62"/>
       <c r="M9" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3438,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="53"/>
-      <c r="R9" s="107"/>
+      <c r="R9" s="62"/>
       <c r="S9" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3450,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="W9" s="53"/>
-      <c r="X9" s="107"/>
+      <c r="X9" s="62"/>
       <c r="Y9" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3462,7 +3372,7 @@
         <v>0</v>
       </c>
       <c r="AC9" s="53"/>
-      <c r="AD9" s="107"/>
+      <c r="AD9" s="62"/>
       <c r="AE9" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3474,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="AI9" s="53"/>
-      <c r="AJ9" s="107"/>
+      <c r="AJ9" s="62"/>
       <c r="AK9" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3489,7 +3399,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="53"/>
-      <c r="F10" s="107"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3501,7 +3411,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="53"/>
-      <c r="L10" s="107"/>
+      <c r="L10" s="62"/>
       <c r="M10" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3513,7 +3423,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="53"/>
-      <c r="R10" s="107"/>
+      <c r="R10" s="62"/>
       <c r="S10" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3525,7 +3435,7 @@
         <v>0</v>
       </c>
       <c r="W10" s="53"/>
-      <c r="X10" s="107"/>
+      <c r="X10" s="62"/>
       <c r="Y10" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3537,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="AC10" s="53"/>
-      <c r="AD10" s="107"/>
+      <c r="AD10" s="62"/>
       <c r="AE10" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3549,7 +3459,7 @@
         <v>0</v>
       </c>
       <c r="AI10" s="53"/>
-      <c r="AJ10" s="107"/>
+      <c r="AJ10" s="62"/>
       <c r="AK10" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3564,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="53"/>
-      <c r="F11" s="107"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3576,7 +3486,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="53"/>
-      <c r="L11" s="107"/>
+      <c r="L11" s="62"/>
       <c r="M11" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3588,7 +3498,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="53"/>
-      <c r="R11" s="107"/>
+      <c r="R11" s="62"/>
       <c r="S11" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3600,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="W11" s="53"/>
-      <c r="X11" s="107"/>
+      <c r="X11" s="62"/>
       <c r="Y11" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3612,7 +3522,7 @@
         <v>0</v>
       </c>
       <c r="AC11" s="53"/>
-      <c r="AD11" s="107"/>
+      <c r="AD11" s="62"/>
       <c r="AE11" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3624,7 +3534,7 @@
         <v>0</v>
       </c>
       <c r="AI11" s="53"/>
-      <c r="AJ11" s="107"/>
+      <c r="AJ11" s="62"/>
       <c r="AK11" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3639,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="53"/>
-      <c r="F12" s="107"/>
+      <c r="F12" s="62"/>
       <c r="G12" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3651,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="53"/>
-      <c r="L12" s="107"/>
+      <c r="L12" s="62"/>
       <c r="M12" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3663,7 +3573,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="53"/>
-      <c r="R12" s="107"/>
+      <c r="R12" s="62"/>
       <c r="S12" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3675,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="W12" s="53"/>
-      <c r="X12" s="107"/>
+      <c r="X12" s="62"/>
       <c r="Y12" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3687,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="AC12" s="53"/>
-      <c r="AD12" s="107"/>
+      <c r="AD12" s="62"/>
       <c r="AE12" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3699,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="AI12" s="53"/>
-      <c r="AJ12" s="107"/>
+      <c r="AJ12" s="62"/>
       <c r="AK12" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3714,7 +3624,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="53"/>
-      <c r="F13" s="107"/>
+      <c r="F13" s="62"/>
       <c r="G13" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3726,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="53"/>
-      <c r="L13" s="107"/>
+      <c r="L13" s="62"/>
       <c r="M13" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3738,7 +3648,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="53"/>
-      <c r="R13" s="107"/>
+      <c r="R13" s="62"/>
       <c r="S13" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3750,7 +3660,7 @@
         <v>0</v>
       </c>
       <c r="W13" s="53"/>
-      <c r="X13" s="107"/>
+      <c r="X13" s="62"/>
       <c r="Y13" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3762,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="AC13" s="53"/>
-      <c r="AD13" s="107"/>
+      <c r="AD13" s="62"/>
       <c r="AE13" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3774,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="AI13" s="53"/>
-      <c r="AJ13" s="107"/>
+      <c r="AJ13" s="62"/>
       <c r="AK13" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3789,7 +3699,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="53"/>
-      <c r="F14" s="107"/>
+      <c r="F14" s="62"/>
       <c r="G14" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3801,7 +3711,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="53"/>
-      <c r="L14" s="107"/>
+      <c r="L14" s="62"/>
       <c r="M14" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3813,7 +3723,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="53"/>
-      <c r="R14" s="107"/>
+      <c r="R14" s="62"/>
       <c r="S14" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3825,7 +3735,7 @@
         <v>0</v>
       </c>
       <c r="W14" s="53"/>
-      <c r="X14" s="107"/>
+      <c r="X14" s="62"/>
       <c r="Y14" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3837,7 +3747,7 @@
         <v>0</v>
       </c>
       <c r="AC14" s="53"/>
-      <c r="AD14" s="107"/>
+      <c r="AD14" s="62"/>
       <c r="AE14" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3849,7 +3759,7 @@
         <v>0</v>
       </c>
       <c r="AI14" s="53"/>
-      <c r="AJ14" s="107"/>
+      <c r="AJ14" s="62"/>
       <c r="AK14" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3864,7 +3774,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="53"/>
-      <c r="F15" s="107"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3876,7 +3786,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="53"/>
-      <c r="L15" s="107"/>
+      <c r="L15" s="62"/>
       <c r="M15" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3888,7 +3798,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="53"/>
-      <c r="R15" s="107"/>
+      <c r="R15" s="62"/>
       <c r="S15" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3900,7 +3810,7 @@
         <v>0</v>
       </c>
       <c r="W15" s="53"/>
-      <c r="X15" s="107"/>
+      <c r="X15" s="62"/>
       <c r="Y15" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3912,7 +3822,7 @@
         <v>0</v>
       </c>
       <c r="AC15" s="53"/>
-      <c r="AD15" s="107"/>
+      <c r="AD15" s="62"/>
       <c r="AE15" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3924,7 +3834,7 @@
         <v>0</v>
       </c>
       <c r="AI15" s="53"/>
-      <c r="AJ15" s="107"/>
+      <c r="AJ15" s="62"/>
       <c r="AK15" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -3939,7 +3849,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="53"/>
-      <c r="F16" s="107"/>
+      <c r="F16" s="62"/>
       <c r="G16" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3951,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="53"/>
-      <c r="L16" s="107"/>
+      <c r="L16" s="62"/>
       <c r="M16" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3963,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="Q16" s="53"/>
-      <c r="R16" s="107"/>
+      <c r="R16" s="62"/>
       <c r="S16" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3975,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="W16" s="53"/>
-      <c r="X16" s="107"/>
+      <c r="X16" s="62"/>
       <c r="Y16" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -3987,7 +3897,7 @@
         <v>0</v>
       </c>
       <c r="AC16" s="53"/>
-      <c r="AD16" s="107"/>
+      <c r="AD16" s="62"/>
       <c r="AE16" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3999,7 +3909,7 @@
         <v>0</v>
       </c>
       <c r="AI16" s="53"/>
-      <c r="AJ16" s="107"/>
+      <c r="AJ16" s="62"/>
       <c r="AK16" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4014,7 +3924,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="53"/>
-      <c r="F17" s="107"/>
+      <c r="F17" s="62"/>
       <c r="G17" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4026,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="53"/>
-      <c r="L17" s="107"/>
+      <c r="L17" s="62"/>
       <c r="M17" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4038,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="53"/>
-      <c r="R17" s="107"/>
+      <c r="R17" s="62"/>
       <c r="S17" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4050,7 +3960,7 @@
         <v>0</v>
       </c>
       <c r="W17" s="53"/>
-      <c r="X17" s="107"/>
+      <c r="X17" s="62"/>
       <c r="Y17" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4062,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="AC17" s="53"/>
-      <c r="AD17" s="107"/>
+      <c r="AD17" s="62"/>
       <c r="AE17" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4074,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="AI17" s="53"/>
-      <c r="AJ17" s="107"/>
+      <c r="AJ17" s="62"/>
       <c r="AK17" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4089,7 +3999,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="53"/>
-      <c r="F18" s="107"/>
+      <c r="F18" s="62"/>
       <c r="G18" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4101,7 +4011,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="53"/>
-      <c r="L18" s="107"/>
+      <c r="L18" s="62"/>
       <c r="M18" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4113,7 +4023,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="53"/>
-      <c r="R18" s="107"/>
+      <c r="R18" s="62"/>
       <c r="S18" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4125,7 +4035,7 @@
         <v>0</v>
       </c>
       <c r="W18" s="53"/>
-      <c r="X18" s="107"/>
+      <c r="X18" s="62"/>
       <c r="Y18" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4137,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="AC18" s="53"/>
-      <c r="AD18" s="107"/>
+      <c r="AD18" s="62"/>
       <c r="AE18" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4149,7 +4059,7 @@
         <v>0</v>
       </c>
       <c r="AI18" s="53"/>
-      <c r="AJ18" s="107"/>
+      <c r="AJ18" s="62"/>
       <c r="AK18" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4164,7 +4074,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="53"/>
-      <c r="F19" s="107"/>
+      <c r="F19" s="62"/>
       <c r="G19" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4176,7 +4086,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="53"/>
-      <c r="L19" s="107"/>
+      <c r="L19" s="62"/>
       <c r="M19" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4188,7 +4098,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="53"/>
-      <c r="R19" s="107"/>
+      <c r="R19" s="62"/>
       <c r="S19" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4200,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="W19" s="53"/>
-      <c r="X19" s="107"/>
+      <c r="X19" s="62"/>
       <c r="Y19" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4212,7 +4122,7 @@
         <v>0</v>
       </c>
       <c r="AC19" s="53"/>
-      <c r="AD19" s="107"/>
+      <c r="AD19" s="62"/>
       <c r="AE19" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4224,7 +4134,7 @@
         <v>0</v>
       </c>
       <c r="AI19" s="53"/>
-      <c r="AJ19" s="107"/>
+      <c r="AJ19" s="62"/>
       <c r="AK19" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4239,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="53"/>
-      <c r="F20" s="107"/>
+      <c r="F20" s="62"/>
       <c r="G20" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4251,7 +4161,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="53"/>
-      <c r="L20" s="107"/>
+      <c r="L20" s="62"/>
       <c r="M20" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4263,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="53"/>
-      <c r="R20" s="107"/>
+      <c r="R20" s="62"/>
       <c r="S20" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4275,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="W20" s="53"/>
-      <c r="X20" s="107"/>
+      <c r="X20" s="62"/>
       <c r="Y20" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4287,7 +4197,7 @@
         <v>0</v>
       </c>
       <c r="AC20" s="53"/>
-      <c r="AD20" s="107"/>
+      <c r="AD20" s="62"/>
       <c r="AE20" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4299,7 +4209,7 @@
         <v>0</v>
       </c>
       <c r="AI20" s="53"/>
-      <c r="AJ20" s="107"/>
+      <c r="AJ20" s="62"/>
       <c r="AK20" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4314,7 +4224,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="53"/>
-      <c r="F21" s="107"/>
+      <c r="F21" s="62"/>
       <c r="G21" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4326,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="53"/>
-      <c r="L21" s="107"/>
+      <c r="L21" s="62"/>
       <c r="M21" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4338,7 +4248,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="53"/>
-      <c r="R21" s="107"/>
+      <c r="R21" s="62"/>
       <c r="S21" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4350,7 +4260,7 @@
         <v>0</v>
       </c>
       <c r="W21" s="53"/>
-      <c r="X21" s="107"/>
+      <c r="X21" s="62"/>
       <c r="Y21" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4362,7 +4272,7 @@
         <v>0</v>
       </c>
       <c r="AC21" s="53"/>
-      <c r="AD21" s="107"/>
+      <c r="AD21" s="62"/>
       <c r="AE21" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4374,7 +4284,7 @@
         <v>0</v>
       </c>
       <c r="AI21" s="53"/>
-      <c r="AJ21" s="107"/>
+      <c r="AJ21" s="62"/>
       <c r="AK21" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4389,7 +4299,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="53"/>
-      <c r="F22" s="107"/>
+      <c r="F22" s="62"/>
       <c r="G22" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4401,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="53"/>
-      <c r="L22" s="107"/>
+      <c r="L22" s="62"/>
       <c r="M22" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4413,7 +4323,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="53"/>
-      <c r="R22" s="107"/>
+      <c r="R22" s="62"/>
       <c r="S22" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4425,7 +4335,7 @@
         <v>0</v>
       </c>
       <c r="W22" s="53"/>
-      <c r="X22" s="107"/>
+      <c r="X22" s="62"/>
       <c r="Y22" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4437,7 +4347,7 @@
         <v>0</v>
       </c>
       <c r="AC22" s="53"/>
-      <c r="AD22" s="107"/>
+      <c r="AD22" s="62"/>
       <c r="AE22" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4449,7 +4359,7 @@
         <v>0</v>
       </c>
       <c r="AI22" s="53"/>
-      <c r="AJ22" s="107"/>
+      <c r="AJ22" s="62"/>
       <c r="AK22" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4464,7 +4374,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="53"/>
-      <c r="F23" s="107"/>
+      <c r="F23" s="62"/>
       <c r="G23" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4476,7 +4386,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="53"/>
-      <c r="L23" s="107"/>
+      <c r="L23" s="62"/>
       <c r="M23" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4488,7 +4398,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="53"/>
-      <c r="R23" s="107"/>
+      <c r="R23" s="62"/>
       <c r="S23" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4500,7 +4410,7 @@
         <v>0</v>
       </c>
       <c r="W23" s="53"/>
-      <c r="X23" s="107"/>
+      <c r="X23" s="62"/>
       <c r="Y23" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4512,7 +4422,7 @@
         <v>0</v>
       </c>
       <c r="AC23" s="53"/>
-      <c r="AD23" s="107"/>
+      <c r="AD23" s="62"/>
       <c r="AE23" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4524,7 +4434,7 @@
         <v>0</v>
       </c>
       <c r="AI23" s="53"/>
-      <c r="AJ23" s="107"/>
+      <c r="AJ23" s="62"/>
       <c r="AK23" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4539,7 +4449,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="53"/>
-      <c r="F24" s="107"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4551,7 +4461,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="53"/>
-      <c r="L24" s="107"/>
+      <c r="L24" s="62"/>
       <c r="M24" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4563,7 +4473,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="53"/>
-      <c r="R24" s="107"/>
+      <c r="R24" s="62"/>
       <c r="S24" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4575,7 +4485,7 @@
         <v>0</v>
       </c>
       <c r="W24" s="53"/>
-      <c r="X24" s="107"/>
+      <c r="X24" s="62"/>
       <c r="Y24" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4587,7 +4497,7 @@
         <v>0</v>
       </c>
       <c r="AC24" s="53"/>
-      <c r="AD24" s="107"/>
+      <c r="AD24" s="62"/>
       <c r="AE24" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4599,7 +4509,7 @@
         <v>0</v>
       </c>
       <c r="AI24" s="53"/>
-      <c r="AJ24" s="107"/>
+      <c r="AJ24" s="62"/>
       <c r="AK24" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4614,7 +4524,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="53"/>
-      <c r="F25" s="107"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4626,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="53"/>
-      <c r="L25" s="107"/>
+      <c r="L25" s="62"/>
       <c r="M25" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4638,7 +4548,7 @@
         <v>0</v>
       </c>
       <c r="Q25" s="53"/>
-      <c r="R25" s="107"/>
+      <c r="R25" s="62"/>
       <c r="S25" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4650,7 +4560,7 @@
         <v>0</v>
       </c>
       <c r="W25" s="53"/>
-      <c r="X25" s="107"/>
+      <c r="X25" s="62"/>
       <c r="Y25" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4662,7 +4572,7 @@
         <v>0</v>
       </c>
       <c r="AC25" s="53"/>
-      <c r="AD25" s="107"/>
+      <c r="AD25" s="62"/>
       <c r="AE25" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4674,7 +4584,7 @@
         <v>0</v>
       </c>
       <c r="AI25" s="53"/>
-      <c r="AJ25" s="107"/>
+      <c r="AJ25" s="62"/>
       <c r="AK25" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4689,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="53"/>
-      <c r="F26" s="107"/>
+      <c r="F26" s="62"/>
       <c r="G26" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4701,7 +4611,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="53"/>
-      <c r="L26" s="107"/>
+      <c r="L26" s="62"/>
       <c r="M26" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4713,7 +4623,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="53"/>
-      <c r="R26" s="107"/>
+      <c r="R26" s="62"/>
       <c r="S26" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4725,7 +4635,7 @@
         <v>0</v>
       </c>
       <c r="W26" s="53"/>
-      <c r="X26" s="107"/>
+      <c r="X26" s="62"/>
       <c r="Y26" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4737,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="AC26" s="53"/>
-      <c r="AD26" s="107"/>
+      <c r="AD26" s="62"/>
       <c r="AE26" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4749,7 +4659,7 @@
         <v>0</v>
       </c>
       <c r="AI26" s="53"/>
-      <c r="AJ26" s="107"/>
+      <c r="AJ26" s="62"/>
       <c r="AK26" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4764,7 +4674,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="53"/>
-      <c r="F27" s="107"/>
+      <c r="F27" s="62"/>
       <c r="G27" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4776,7 +4686,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="53"/>
-      <c r="L27" s="107"/>
+      <c r="L27" s="62"/>
       <c r="M27" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4788,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="53"/>
-      <c r="R27" s="107"/>
+      <c r="R27" s="62"/>
       <c r="S27" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4800,7 +4710,7 @@
         <v>0</v>
       </c>
       <c r="W27" s="53"/>
-      <c r="X27" s="107"/>
+      <c r="X27" s="62"/>
       <c r="Y27" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4812,7 +4722,7 @@
         <v>0</v>
       </c>
       <c r="AC27" s="53"/>
-      <c r="AD27" s="107"/>
+      <c r="AD27" s="62"/>
       <c r="AE27" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4824,7 +4734,7 @@
         <v>0</v>
       </c>
       <c r="AI27" s="53"/>
-      <c r="AJ27" s="107"/>
+      <c r="AJ27" s="62"/>
       <c r="AK27" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4839,7 +4749,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="53"/>
-      <c r="F28" s="107"/>
+      <c r="F28" s="62"/>
       <c r="G28" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4851,7 +4761,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="53"/>
-      <c r="L28" s="107"/>
+      <c r="L28" s="62"/>
       <c r="M28" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4863,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="53"/>
-      <c r="R28" s="107"/>
+      <c r="R28" s="62"/>
       <c r="S28" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4875,7 +4785,7 @@
         <v>0</v>
       </c>
       <c r="W28" s="53"/>
-      <c r="X28" s="107"/>
+      <c r="X28" s="62"/>
       <c r="Y28" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4887,7 +4797,7 @@
         <v>0</v>
       </c>
       <c r="AC28" s="53"/>
-      <c r="AD28" s="107"/>
+      <c r="AD28" s="62"/>
       <c r="AE28" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4899,7 +4809,7 @@
         <v>0</v>
       </c>
       <c r="AI28" s="53"/>
-      <c r="AJ28" s="107"/>
+      <c r="AJ28" s="62"/>
       <c r="AK28" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4914,7 +4824,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="53"/>
-      <c r="F29" s="107"/>
+      <c r="F29" s="62"/>
       <c r="G29" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4926,7 +4836,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="53"/>
-      <c r="L29" s="107"/>
+      <c r="L29" s="62"/>
       <c r="M29" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4938,7 +4848,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="53"/>
-      <c r="R29" s="107"/>
+      <c r="R29" s="62"/>
       <c r="S29" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4950,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="W29" s="53"/>
-      <c r="X29" s="107"/>
+      <c r="X29" s="62"/>
       <c r="Y29" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4962,7 +4872,7 @@
         <v>0</v>
       </c>
       <c r="AC29" s="53"/>
-      <c r="AD29" s="107"/>
+      <c r="AD29" s="62"/>
       <c r="AE29" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4974,7 +4884,7 @@
         <v>0</v>
       </c>
       <c r="AI29" s="53"/>
-      <c r="AJ29" s="107"/>
+      <c r="AJ29" s="62"/>
       <c r="AK29" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -4989,7 +4899,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="53"/>
-      <c r="F30" s="107"/>
+      <c r="F30" s="62"/>
       <c r="G30" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5001,7 +4911,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="53"/>
-      <c r="L30" s="107"/>
+      <c r="L30" s="62"/>
       <c r="M30" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5013,7 +4923,7 @@
         <v>0</v>
       </c>
       <c r="Q30" s="53"/>
-      <c r="R30" s="107"/>
+      <c r="R30" s="62"/>
       <c r="S30" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5025,7 +4935,7 @@
         <v>0</v>
       </c>
       <c r="W30" s="53"/>
-      <c r="X30" s="107"/>
+      <c r="X30" s="62"/>
       <c r="Y30" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5037,7 +4947,7 @@
         <v>0</v>
       </c>
       <c r="AC30" s="53"/>
-      <c r="AD30" s="107"/>
+      <c r="AD30" s="62"/>
       <c r="AE30" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5049,7 +4959,7 @@
         <v>0</v>
       </c>
       <c r="AI30" s="53"/>
-      <c r="AJ30" s="107"/>
+      <c r="AJ30" s="62"/>
       <c r="AK30" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5064,7 +4974,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="53"/>
-      <c r="F31" s="107"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5076,7 +4986,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="53"/>
-      <c r="L31" s="107"/>
+      <c r="L31" s="62"/>
       <c r="M31" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5088,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="Q31" s="53"/>
-      <c r="R31" s="107"/>
+      <c r="R31" s="62"/>
       <c r="S31" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5100,7 +5010,7 @@
         <v>0</v>
       </c>
       <c r="W31" s="53"/>
-      <c r="X31" s="107"/>
+      <c r="X31" s="62"/>
       <c r="Y31" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5112,7 +5022,7 @@
         <v>0</v>
       </c>
       <c r="AC31" s="53"/>
-      <c r="AD31" s="107"/>
+      <c r="AD31" s="62"/>
       <c r="AE31" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5124,7 +5034,7 @@
         <v>0</v>
       </c>
       <c r="AI31" s="53"/>
-      <c r="AJ31" s="107"/>
+      <c r="AJ31" s="62"/>
       <c r="AK31" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5139,7 +5049,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="53"/>
-      <c r="F32" s="107"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5151,7 +5061,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="53"/>
-      <c r="L32" s="107"/>
+      <c r="L32" s="62"/>
       <c r="M32" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5163,7 +5073,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="53"/>
-      <c r="R32" s="107"/>
+      <c r="R32" s="62"/>
       <c r="S32" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5175,7 +5085,7 @@
         <v>0</v>
       </c>
       <c r="W32" s="53"/>
-      <c r="X32" s="107"/>
+      <c r="X32" s="62"/>
       <c r="Y32" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5187,7 +5097,7 @@
         <v>0</v>
       </c>
       <c r="AC32" s="53"/>
-      <c r="AD32" s="107"/>
+      <c r="AD32" s="62"/>
       <c r="AE32" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5199,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="AI32" s="53"/>
-      <c r="AJ32" s="107"/>
+      <c r="AJ32" s="62"/>
       <c r="AK32" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5214,7 +5124,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="53"/>
-      <c r="F33" s="107"/>
+      <c r="F33" s="62"/>
       <c r="G33" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5226,7 +5136,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="53"/>
-      <c r="L33" s="107"/>
+      <c r="L33" s="62"/>
       <c r="M33" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5238,7 +5148,7 @@
         <v>0</v>
       </c>
       <c r="Q33" s="53"/>
-      <c r="R33" s="107"/>
+      <c r="R33" s="62"/>
       <c r="S33" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5250,7 +5160,7 @@
         <v>0</v>
       </c>
       <c r="W33" s="53"/>
-      <c r="X33" s="107"/>
+      <c r="X33" s="62"/>
       <c r="Y33" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5262,7 +5172,7 @@
         <v>0</v>
       </c>
       <c r="AC33" s="53"/>
-      <c r="AD33" s="107"/>
+      <c r="AD33" s="62"/>
       <c r="AE33" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5274,7 +5184,7 @@
         <v>0</v>
       </c>
       <c r="AI33" s="53"/>
-      <c r="AJ33" s="107"/>
+      <c r="AJ33" s="62"/>
       <c r="AK33" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5289,7 +5199,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="53"/>
-      <c r="F34" s="107"/>
+      <c r="F34" s="62"/>
       <c r="G34" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5301,7 +5211,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="53"/>
-      <c r="L34" s="107"/>
+      <c r="L34" s="62"/>
       <c r="M34" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5313,7 +5223,7 @@
         <v>0</v>
       </c>
       <c r="Q34" s="53"/>
-      <c r="R34" s="107"/>
+      <c r="R34" s="62"/>
       <c r="S34" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5325,7 +5235,7 @@
         <v>0</v>
       </c>
       <c r="W34" s="53"/>
-      <c r="X34" s="107"/>
+      <c r="X34" s="62"/>
       <c r="Y34" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5337,7 +5247,7 @@
         <v>0</v>
       </c>
       <c r="AC34" s="53"/>
-      <c r="AD34" s="107"/>
+      <c r="AD34" s="62"/>
       <c r="AE34" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5349,7 +5259,7 @@
         <v>0</v>
       </c>
       <c r="AI34" s="53"/>
-      <c r="AJ34" s="107"/>
+      <c r="AJ34" s="62"/>
       <c r="AK34" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5364,7 +5274,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="53"/>
-      <c r="F35" s="107"/>
+      <c r="F35" s="62"/>
       <c r="G35" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5376,7 +5286,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="53"/>
-      <c r="L35" s="107"/>
+      <c r="L35" s="62"/>
       <c r="M35" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5388,7 +5298,7 @@
         <v>0</v>
       </c>
       <c r="Q35" s="53"/>
-      <c r="R35" s="107"/>
+      <c r="R35" s="62"/>
       <c r="S35" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5400,7 +5310,7 @@
         <v>0</v>
       </c>
       <c r="W35" s="53"/>
-      <c r="X35" s="107"/>
+      <c r="X35" s="62"/>
       <c r="Y35" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5412,7 +5322,7 @@
         <v>0</v>
       </c>
       <c r="AC35" s="53"/>
-      <c r="AD35" s="107"/>
+      <c r="AD35" s="62"/>
       <c r="AE35" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5424,7 +5334,7 @@
         <v>0</v>
       </c>
       <c r="AI35" s="53"/>
-      <c r="AJ35" s="107"/>
+      <c r="AJ35" s="62"/>
       <c r="AK35" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5439,7 +5349,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="53"/>
-      <c r="F36" s="107"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5451,7 +5361,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="53"/>
-      <c r="L36" s="107"/>
+      <c r="L36" s="62"/>
       <c r="M36" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5463,7 +5373,7 @@
         <v>0</v>
       </c>
       <c r="Q36" s="53"/>
-      <c r="R36" s="107"/>
+      <c r="R36" s="62"/>
       <c r="S36" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5475,7 +5385,7 @@
         <v>0</v>
       </c>
       <c r="W36" s="53"/>
-      <c r="X36" s="107"/>
+      <c r="X36" s="62"/>
       <c r="Y36" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5487,7 +5397,7 @@
         <v>0</v>
       </c>
       <c r="AC36" s="53"/>
-      <c r="AD36" s="107"/>
+      <c r="AD36" s="62"/>
       <c r="AE36" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5499,7 +5409,7 @@
         <v>0</v>
       </c>
       <c r="AI36" s="53"/>
-      <c r="AJ36" s="107"/>
+      <c r="AJ36" s="62"/>
       <c r="AK36" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5514,7 +5424,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="53"/>
-      <c r="F37" s="107"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5526,7 +5436,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="53"/>
-      <c r="L37" s="107"/>
+      <c r="L37" s="62"/>
       <c r="M37" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5538,7 +5448,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="53"/>
-      <c r="R37" s="107"/>
+      <c r="R37" s="62"/>
       <c r="S37" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5550,7 +5460,7 @@
         <v>0</v>
       </c>
       <c r="W37" s="53"/>
-      <c r="X37" s="107"/>
+      <c r="X37" s="62"/>
       <c r="Y37" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5562,7 +5472,7 @@
         <v>0</v>
       </c>
       <c r="AC37" s="53"/>
-      <c r="AD37" s="107"/>
+      <c r="AD37" s="62"/>
       <c r="AE37" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5574,7 +5484,7 @@
         <v>0</v>
       </c>
       <c r="AI37" s="53"/>
-      <c r="AJ37" s="107"/>
+      <c r="AJ37" s="62"/>
       <c r="AK37" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5589,7 +5499,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="53"/>
-      <c r="F38" s="107"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5601,7 +5511,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="53"/>
-      <c r="L38" s="107"/>
+      <c r="L38" s="62"/>
       <c r="M38" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5613,7 +5523,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="53"/>
-      <c r="R38" s="107"/>
+      <c r="R38" s="62"/>
       <c r="S38" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5625,7 +5535,7 @@
         <v>0</v>
       </c>
       <c r="W38" s="53"/>
-      <c r="X38" s="107"/>
+      <c r="X38" s="62"/>
       <c r="Y38" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5637,7 +5547,7 @@
         <v>0</v>
       </c>
       <c r="AC38" s="53"/>
-      <c r="AD38" s="107"/>
+      <c r="AD38" s="62"/>
       <c r="AE38" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5649,7 +5559,7 @@
         <v>0</v>
       </c>
       <c r="AI38" s="53"/>
-      <c r="AJ38" s="107"/>
+      <c r="AJ38" s="62"/>
       <c r="AK38" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5664,7 +5574,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="53"/>
-      <c r="F39" s="107"/>
+      <c r="F39" s="62"/>
       <c r="G39" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5676,7 +5586,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="53"/>
-      <c r="L39" s="107"/>
+      <c r="L39" s="62"/>
       <c r="M39" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5688,7 +5598,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="53"/>
-      <c r="R39" s="107"/>
+      <c r="R39" s="62"/>
       <c r="S39" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5700,7 +5610,7 @@
         <v>0</v>
       </c>
       <c r="W39" s="53"/>
-      <c r="X39" s="107"/>
+      <c r="X39" s="62"/>
       <c r="Y39" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5712,7 +5622,7 @@
         <v>0</v>
       </c>
       <c r="AC39" s="53"/>
-      <c r="AD39" s="107"/>
+      <c r="AD39" s="62"/>
       <c r="AE39" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5724,7 +5634,7 @@
         <v>0</v>
       </c>
       <c r="AI39" s="53"/>
-      <c r="AJ39" s="107"/>
+      <c r="AJ39" s="62"/>
       <c r="AK39" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5739,7 +5649,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="53"/>
-      <c r="F40" s="107"/>
+      <c r="F40" s="62"/>
       <c r="G40" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5751,7 +5661,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="53"/>
-      <c r="L40" s="107"/>
+      <c r="L40" s="62"/>
       <c r="M40" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5763,7 +5673,7 @@
         <v>0</v>
       </c>
       <c r="Q40" s="53"/>
-      <c r="R40" s="107"/>
+      <c r="R40" s="62"/>
       <c r="S40" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5775,7 +5685,7 @@
         <v>0</v>
       </c>
       <c r="W40" s="53"/>
-      <c r="X40" s="107"/>
+      <c r="X40" s="62"/>
       <c r="Y40" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5787,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="AC40" s="53"/>
-      <c r="AD40" s="107"/>
+      <c r="AD40" s="62"/>
       <c r="AE40" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5799,7 +5709,7 @@
         <v>0</v>
       </c>
       <c r="AI40" s="53"/>
-      <c r="AJ40" s="107"/>
+      <c r="AJ40" s="62"/>
       <c r="AK40" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5814,7 +5724,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="53"/>
-      <c r="F41" s="107"/>
+      <c r="F41" s="62"/>
       <c r="G41" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5826,7 +5736,7 @@
         <v>0</v>
       </c>
       <c r="K41" s="53"/>
-      <c r="L41" s="107"/>
+      <c r="L41" s="62"/>
       <c r="M41" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5838,7 +5748,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="53"/>
-      <c r="R41" s="107"/>
+      <c r="R41" s="62"/>
       <c r="S41" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5850,7 +5760,7 @@
         <v>0</v>
       </c>
       <c r="W41" s="53"/>
-      <c r="X41" s="107"/>
+      <c r="X41" s="62"/>
       <c r="Y41" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5862,7 +5772,7 @@
         <v>0</v>
       </c>
       <c r="AC41" s="53"/>
-      <c r="AD41" s="107"/>
+      <c r="AD41" s="62"/>
       <c r="AE41" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5874,7 +5784,7 @@
         <v>0</v>
       </c>
       <c r="AI41" s="53"/>
-      <c r="AJ41" s="107"/>
+      <c r="AJ41" s="62"/>
       <c r="AK41" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5889,7 +5799,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="53"/>
-      <c r="F42" s="107"/>
+      <c r="F42" s="62"/>
       <c r="G42" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5901,7 +5811,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="53"/>
-      <c r="L42" s="107"/>
+      <c r="L42" s="62"/>
       <c r="M42" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5913,7 +5823,7 @@
         <v>0</v>
       </c>
       <c r="Q42" s="53"/>
-      <c r="R42" s="107"/>
+      <c r="R42" s="62"/>
       <c r="S42" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5925,7 +5835,7 @@
         <v>0</v>
       </c>
       <c r="W42" s="53"/>
-      <c r="X42" s="107"/>
+      <c r="X42" s="62"/>
       <c r="Y42" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5937,7 +5847,7 @@
         <v>0</v>
       </c>
       <c r="AC42" s="53"/>
-      <c r="AD42" s="107"/>
+      <c r="AD42" s="62"/>
       <c r="AE42" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -5949,7 +5859,7 @@
         <v>0</v>
       </c>
       <c r="AI42" s="53"/>
-      <c r="AJ42" s="107"/>
+      <c r="AJ42" s="62"/>
       <c r="AK42" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -5964,7 +5874,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="53"/>
-      <c r="F43" s="107"/>
+      <c r="F43" s="62"/>
       <c r="G43" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5976,7 +5886,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="53"/>
-      <c r="L43" s="107"/>
+      <c r="L43" s="62"/>
       <c r="M43" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5988,7 +5898,7 @@
         <v>0</v>
       </c>
       <c r="Q43" s="53"/>
-      <c r="R43" s="107"/>
+      <c r="R43" s="62"/>
       <c r="S43" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6000,7 +5910,7 @@
         <v>0</v>
       </c>
       <c r="W43" s="53"/>
-      <c r="X43" s="107"/>
+      <c r="X43" s="62"/>
       <c r="Y43" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6012,7 +5922,7 @@
         <v>0</v>
       </c>
       <c r="AC43" s="53"/>
-      <c r="AD43" s="107"/>
+      <c r="AD43" s="62"/>
       <c r="AE43" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6024,7 +5934,7 @@
         <v>0</v>
       </c>
       <c r="AI43" s="53"/>
-      <c r="AJ43" s="107"/>
+      <c r="AJ43" s="62"/>
       <c r="AK43" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -6039,7 +5949,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="53"/>
-      <c r="F44" s="107"/>
+      <c r="F44" s="62"/>
       <c r="G44" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6051,7 +5961,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="53"/>
-      <c r="L44" s="107"/>
+      <c r="L44" s="62"/>
       <c r="M44" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6063,7 +5973,7 @@
         <v>0</v>
       </c>
       <c r="Q44" s="53"/>
-      <c r="R44" s="107"/>
+      <c r="R44" s="62"/>
       <c r="S44" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6075,7 +5985,7 @@
         <v>0</v>
       </c>
       <c r="W44" s="53"/>
-      <c r="X44" s="107"/>
+      <c r="X44" s="62"/>
       <c r="Y44" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6087,7 +5997,7 @@
         <v>0</v>
       </c>
       <c r="AC44" s="53"/>
-      <c r="AD44" s="107"/>
+      <c r="AD44" s="62"/>
       <c r="AE44" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6099,7 +6009,7 @@
         <v>0</v>
       </c>
       <c r="AI44" s="53"/>
-      <c r="AJ44" s="107"/>
+      <c r="AJ44" s="62"/>
       <c r="AK44" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -6114,7 +6024,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="53"/>
-      <c r="F45" s="107"/>
+      <c r="F45" s="62"/>
       <c r="G45" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6126,7 +6036,7 @@
         <v>0</v>
       </c>
       <c r="K45" s="53"/>
-      <c r="L45" s="107"/>
+      <c r="L45" s="62"/>
       <c r="M45" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6138,7 +6048,7 @@
         <v>0</v>
       </c>
       <c r="Q45" s="53"/>
-      <c r="R45" s="107"/>
+      <c r="R45" s="62"/>
       <c r="S45" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6150,7 +6060,7 @@
         <v>0</v>
       </c>
       <c r="W45" s="53"/>
-      <c r="X45" s="107"/>
+      <c r="X45" s="62"/>
       <c r="Y45" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6162,7 +6072,7 @@
         <v>0</v>
       </c>
       <c r="AC45" s="53"/>
-      <c r="AD45" s="107"/>
+      <c r="AD45" s="62"/>
       <c r="AE45" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6174,7 +6084,7 @@
         <v>0</v>
       </c>
       <c r="AI45" s="53"/>
-      <c r="AJ45" s="107"/>
+      <c r="AJ45" s="62"/>
       <c r="AK45" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -6189,7 +6099,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="53"/>
-      <c r="F46" s="107"/>
+      <c r="F46" s="62"/>
       <c r="G46" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6201,7 +6111,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="53"/>
-      <c r="L46" s="107"/>
+      <c r="L46" s="62"/>
       <c r="M46" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6213,7 +6123,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="53"/>
-      <c r="R46" s="107"/>
+      <c r="R46" s="62"/>
       <c r="S46" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6225,7 +6135,7 @@
         <v>0</v>
       </c>
       <c r="W46" s="53"/>
-      <c r="X46" s="107"/>
+      <c r="X46" s="62"/>
       <c r="Y46" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6237,7 +6147,7 @@
         <v>0</v>
       </c>
       <c r="AC46" s="53"/>
-      <c r="AD46" s="107"/>
+      <c r="AD46" s="62"/>
       <c r="AE46" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6249,7 +6159,7 @@
         <v>0</v>
       </c>
       <c r="AI46" s="53"/>
-      <c r="AJ46" s="107"/>
+      <c r="AJ46" s="62"/>
       <c r="AK46" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -6264,7 +6174,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="53"/>
-      <c r="F47" s="107"/>
+      <c r="F47" s="62"/>
       <c r="G47" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6276,7 +6186,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="53"/>
-      <c r="L47" s="107"/>
+      <c r="L47" s="62"/>
       <c r="M47" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6288,7 +6198,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="53"/>
-      <c r="R47" s="107"/>
+      <c r="R47" s="62"/>
       <c r="S47" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6300,7 +6210,7 @@
         <v>0</v>
       </c>
       <c r="W47" s="53"/>
-      <c r="X47" s="107"/>
+      <c r="X47" s="62"/>
       <c r="Y47" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6312,7 +6222,7 @@
         <v>0</v>
       </c>
       <c r="AC47" s="53"/>
-      <c r="AD47" s="107"/>
+      <c r="AD47" s="62"/>
       <c r="AE47" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6324,7 +6234,7 @@
         <v>0</v>
       </c>
       <c r="AI47" s="53"/>
-      <c r="AJ47" s="107"/>
+      <c r="AJ47" s="62"/>
       <c r="AK47" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -6339,7 +6249,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="53"/>
-      <c r="F48" s="107"/>
+      <c r="F48" s="62"/>
       <c r="G48" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6351,7 +6261,7 @@
         <v>0</v>
       </c>
       <c r="K48" s="53"/>
-      <c r="L48" s="107"/>
+      <c r="L48" s="62"/>
       <c r="M48" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6363,7 +6273,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="53"/>
-      <c r="R48" s="107"/>
+      <c r="R48" s="62"/>
       <c r="S48" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6375,7 +6285,7 @@
         <v>0</v>
       </c>
       <c r="W48" s="53"/>
-      <c r="X48" s="107"/>
+      <c r="X48" s="62"/>
       <c r="Y48" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6387,7 +6297,7 @@
         <v>0</v>
       </c>
       <c r="AC48" s="53"/>
-      <c r="AD48" s="107"/>
+      <c r="AD48" s="62"/>
       <c r="AE48" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6399,7 +6309,7 @@
         <v>0</v>
       </c>
       <c r="AI48" s="53"/>
-      <c r="AJ48" s="107"/>
+      <c r="AJ48" s="62"/>
       <c r="AK48" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -6414,7 +6324,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="56"/>
-      <c r="F49" s="108"/>
+      <c r="F49" s="63"/>
       <c r="G49" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6426,7 +6336,7 @@
         <v>0</v>
       </c>
       <c r="K49" s="56"/>
-      <c r="L49" s="108"/>
+      <c r="L49" s="63"/>
       <c r="M49" s="50">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6438,7 +6348,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="56"/>
-      <c r="R49" s="108"/>
+      <c r="R49" s="63"/>
       <c r="S49" s="50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -6450,7 +6360,7 @@
         <v>0</v>
       </c>
       <c r="W49" s="56"/>
-      <c r="X49" s="108"/>
+      <c r="X49" s="63"/>
       <c r="Y49" s="50">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -6462,7 +6372,7 @@
         <v>0</v>
       </c>
       <c r="AC49" s="56"/>
-      <c r="AD49" s="108"/>
+      <c r="AD49" s="63"/>
       <c r="AE49" s="50">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6474,7 +6384,7 @@
         <v>0</v>
       </c>
       <c r="AI49" s="56"/>
-      <c r="AJ49" s="108"/>
+      <c r="AJ49" s="63"/>
       <c r="AK49" s="50">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -6497,7 +6407,7 @@
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="F50" s="109">
+      <c r="F50" s="64">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
@@ -6521,7 +6431,7 @@
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="L50" s="109">
+      <c r="L50" s="64">
         <f t="shared" ref="L50" si="32">SUM(L4:L49)</f>
         <v>0</v>
       </c>
@@ -6545,7 +6455,7 @@
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="R50" s="109">
+      <c r="R50" s="64">
         <f t="shared" ref="R50" si="35">SUM(R4:R49)</f>
         <v>0</v>
       </c>
@@ -6569,7 +6479,7 @@
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="X50" s="109">
+      <c r="X50" s="64">
         <f t="shared" ref="X50" si="38">SUM(X4:X49)</f>
         <v>0</v>
       </c>
@@ -6593,7 +6503,7 @@
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AD50" s="109">
+      <c r="AD50" s="64">
         <f t="shared" ref="AD50" si="41">SUM(AD4:AD49)</f>
         <v>0</v>
       </c>
@@ -6617,7 +6527,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AJ50" s="109">
+      <c r="AJ50" s="64">
         <f t="shared" ref="AJ50" si="44">SUM(AJ4:AJ49)</f>
         <v>0</v>
       </c>
@@ -6639,55 +6549,55 @@
     <mergeCell ref="T2:Y2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:F49">
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G50 M4:M50 S4:S50 Y4:Y50 AE4:AE50 AK4:AK50">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:L49">
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:R49">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:X49">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4:AD49">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH4:AJ49">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G50 M4:M50 S4:S50 Y4:Y50 AE4:AE50 AK4:AK50">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6756,136 +6666,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="90"/>
     </row>
     <row r="2" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="70" t="s">
+      <c r="B2" s="92"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="70" t="s">
+      <c r="E2" s="92"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="72"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="75"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="96"/>
     </row>
     <row r="4" spans="1:46" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="78"/>
+      <c r="A4" s="97"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="99"/>
     </row>
     <row r="5" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="82" t="s">
+      <c r="B5" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="64" t="s">
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="64" t="s">
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="65"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="64" t="s">
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="65"/>
-      <c r="Z5" s="65"/>
-      <c r="AA5" s="65"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="64" t="s">
+      <c r="X5" s="79"/>
+      <c r="Y5" s="79"/>
+      <c r="Z5" s="79"/>
+      <c r="AA5" s="79"/>
+      <c r="AB5" s="80"/>
+      <c r="AC5" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="AD5" s="65"/>
-      <c r="AE5" s="65"/>
-      <c r="AF5" s="65"/>
-      <c r="AG5" s="65"/>
-      <c r="AH5" s="66"/>
-      <c r="AI5" s="64" t="s">
+      <c r="AD5" s="79"/>
+      <c r="AE5" s="79"/>
+      <c r="AF5" s="79"/>
+      <c r="AG5" s="79"/>
+      <c r="AH5" s="80"/>
+      <c r="AI5" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="AJ5" s="65"/>
-      <c r="AK5" s="65"/>
-      <c r="AL5" s="65"/>
-      <c r="AM5" s="65"/>
-      <c r="AN5" s="66"/>
-      <c r="AO5" s="64" t="s">
+      <c r="AJ5" s="79"/>
+      <c r="AK5" s="79"/>
+      <c r="AL5" s="79"/>
+      <c r="AM5" s="79"/>
+      <c r="AN5" s="80"/>
+      <c r="AO5" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="AP5" s="65"/>
-      <c r="AQ5" s="65"/>
-      <c r="AR5" s="65"/>
-      <c r="AS5" s="65"/>
-      <c r="AT5" s="66"/>
+      <c r="AP5" s="79"/>
+      <c r="AQ5" s="79"/>
+      <c r="AR5" s="79"/>
+      <c r="AS5" s="79"/>
+      <c r="AT5" s="80"/>
     </row>
     <row r="6" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="81"/>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="85"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="86"/>
       <c r="E6" s="10" t="s">
         <v>15</v>
       </c>
@@ -7062,10 +6972,10 @@
       <c r="AT7" s="7"/>
     </row>
     <row r="8" spans="1:46" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -7110,80 +7020,80 @@
       <c r="AT8" s="8"/>
     </row>
     <row r="9" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="82" t="s">
+      <c r="B9" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="82" t="s">
+      <c r="D9" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="64" t="s">
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="64" t="s">
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="R9" s="65"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="65"/>
-      <c r="U9" s="65"/>
-      <c r="V9" s="66"/>
-      <c r="W9" s="64" t="s">
+      <c r="R9" s="79"/>
+      <c r="S9" s="79"/>
+      <c r="T9" s="79"/>
+      <c r="U9" s="79"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="X9" s="65"/>
-      <c r="Y9" s="65"/>
-      <c r="Z9" s="65"/>
-      <c r="AA9" s="65"/>
-      <c r="AB9" s="66"/>
-      <c r="AC9" s="64" t="s">
+      <c r="X9" s="79"/>
+      <c r="Y9" s="79"/>
+      <c r="Z9" s="79"/>
+      <c r="AA9" s="79"/>
+      <c r="AB9" s="80"/>
+      <c r="AC9" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="AD9" s="65"/>
-      <c r="AE9" s="65"/>
-      <c r="AF9" s="65"/>
-      <c r="AG9" s="65"/>
-      <c r="AH9" s="66"/>
-      <c r="AI9" s="64" t="s">
+      <c r="AD9" s="79"/>
+      <c r="AE9" s="79"/>
+      <c r="AF9" s="79"/>
+      <c r="AG9" s="79"/>
+      <c r="AH9" s="80"/>
+      <c r="AI9" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="AJ9" s="65"/>
-      <c r="AK9" s="65"/>
-      <c r="AL9" s="65"/>
-      <c r="AM9" s="65"/>
-      <c r="AN9" s="66"/>
-      <c r="AO9" s="64" t="s">
+      <c r="AJ9" s="79"/>
+      <c r="AK9" s="79"/>
+      <c r="AL9" s="79"/>
+      <c r="AM9" s="79"/>
+      <c r="AN9" s="80"/>
+      <c r="AO9" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="AP9" s="65"/>
-      <c r="AQ9" s="65"/>
-      <c r="AR9" s="65"/>
-      <c r="AS9" s="65"/>
-      <c r="AT9" s="66"/>
+      <c r="AP9" s="79"/>
+      <c r="AQ9" s="79"/>
+      <c r="AR9" s="79"/>
+      <c r="AS9" s="79"/>
+      <c r="AT9" s="80"/>
     </row>
     <row r="10" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="81"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
       <c r="E10" s="10" t="s">
         <v>15</v>
       </c>
@@ -7360,10 +7270,10 @@
       <c r="AT11" s="7"/>
     </row>
     <row r="12" spans="1:46" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="79"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -7440,14 +7350,14 @@
       <c r="A18" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
-      <c r="G18" s="92"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="74"/>
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
@@ -7459,14 +7369,14 @@
       <c r="A19" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="93" t="s">
+      <c r="B19" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="94"/>
-      <c r="G19" s="95"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="77"/>
       <c r="K19" s="28"/>
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
@@ -7475,42 +7385,42 @@
       <c r="A20" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="93" t="s">
+      <c r="B20" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="94"/>
-      <c r="G20" s="95"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="77"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="93" t="s">
+      <c r="B21" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="95"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="77"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="89"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="89"/>
-      <c r="I22" s="89"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
@@ -7525,51 +7435,51 @@
       <c r="A24" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="88"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="AC5:AH5"/>
+    <mergeCell ref="AC9:AH9"/>
+    <mergeCell ref="AI5:AN5"/>
+    <mergeCell ref="AI9:AN9"/>
+    <mergeCell ref="AO5:AT5"/>
+    <mergeCell ref="AO9:AT9"/>
+    <mergeCell ref="K9:P9"/>
+    <mergeCell ref="Q5:V5"/>
+    <mergeCell ref="Q9:V9"/>
+    <mergeCell ref="W5:AB5"/>
+    <mergeCell ref="W9:AB9"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C4"/>
+    <mergeCell ref="D2:F4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="G2:J4"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B22:I22"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B21:G21"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C4"/>
-    <mergeCell ref="D2:F4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="G2:J4"/>
-    <mergeCell ref="K9:P9"/>
-    <mergeCell ref="Q5:V5"/>
-    <mergeCell ref="Q9:V9"/>
-    <mergeCell ref="W5:AB5"/>
-    <mergeCell ref="W9:AB9"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="AC5:AH5"/>
-    <mergeCell ref="AC9:AH9"/>
-    <mergeCell ref="AI5:AN5"/>
-    <mergeCell ref="AI9:AN9"/>
-    <mergeCell ref="AO5:AT5"/>
-    <mergeCell ref="AO9:AT9"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.23622047244094491" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="45" orientation="landscape" r:id="rId1"/>
@@ -7601,24 +7511,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="98"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="102"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="98"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="102"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -7713,16 +7623,16 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="102" t="s">
+      <c r="B9" s="104"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="100"/>
-      <c r="F9" s="101"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="105"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -7771,16 +7681,16 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="103"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="102" t="s">
+      <c r="B13" s="107"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="100"/>
-      <c r="F13" s="101"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="105"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
@@ -7882,70 +7792,70 @@
       <c r="A22" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="90" t="s">
+      <c r="B22" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="92"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="74"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="93" t="s">
+      <c r="B23" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="95"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="77"/>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="93" t="s">
+      <c r="B24" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="94"/>
-      <c r="D24" s="94"/>
-      <c r="E24" s="94"/>
-      <c r="F24" s="94"/>
-      <c r="G24" s="95"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="77"/>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="93" t="s">
+      <c r="B25" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="94"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="95"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="77"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="105" t="s">
+      <c r="B26" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="88"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="70"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7962,14 +7872,14 @@
       <c r="A28" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="86" t="s">
+      <c r="B28" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="88"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Ajuste na função de criação das abas semanais [AGERGS]
</commit_message>
<xml_diff>
--- a/Modelo_PDO.xlsx
+++ b/Modelo_PDO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70ac05f72bfee68d/Documentos/GUAIBA/Python/ERG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD637E1-B1AE-4745-9C24-AB7A4DFFDC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{1FD637E1-B1AE-4745-9C24-AB7A4DFFDC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E068AB17-E1DE-4190-9669-975D899AFB73}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1340,36 +1340,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1377,27 +1347,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1432,6 +1381,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1466,7 +1466,112 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2390,43 +2495,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1382" displayName="Tabela1382" ref="A10:F11" insertRow="1" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1382" displayName="Tabela1382" ref="A10:F11" insertRow="1" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A10:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DIAS ÚTEIS" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SABADOS " dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DIAS ÚTEIS2" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SABADOS 2" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DIAS ÚTEIS" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SABADOS " dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DIAS ÚTEIS2" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SABADOS 2" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela13493" displayName="Tabela13493" ref="A14:F15" insertRow="1" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela13493" displayName="Tabela13493" ref="A14:F15" insertRow="1" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A14:F15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DIAS ÚTEIS" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SABADOS " dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DIAS ÚTEIS2" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="SABADOS 2" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DIAS ÚTEIS" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SABADOS " dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DIAS ÚTEIS2" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="SABADOS 2" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela94" displayName="Tabela94" ref="A4:D7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela94" displayName="Tabela94" ref="A4:D7" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="A4:D7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="####" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Total de Viagens Oficiais " dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Total de Viagens Extras" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Km's Totais" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="####" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Total de Viagens Oficiais " dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Total de Viagens Extras" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Km's Totais" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2724,8 +2829,8 @@
   </sheetPr>
   <dimension ref="A1:AK50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO27" sqref="AO27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6549,55 +6654,60 @@
     <mergeCell ref="T2:Y2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:F49">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G50 M4:M50 S4:S50 Y4:Y50 AE4:AE50 AK4:AK50">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:L49">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:R49">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:X49">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4:AD49">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH4:AJ49">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G50 M4:M50 S4:S50 Y4:Y50 AE4:AE50 AK4:AK50">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6611,7 +6721,7 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:AT24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -6666,136 +6776,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="90"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="73"/>
     </row>
     <row r="2" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="91" t="s">
+      <c r="B2" s="75"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="92"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="91" t="s">
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="93"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="96"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
     </row>
     <row r="4" spans="1:46" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="97"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="99"/>
+      <c r="A4" s="80"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="83" t="s">
+      <c r="B5" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="78" t="s">
+      <c r="E5" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="78" t="s">
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="80"/>
-      <c r="Q5" s="78" t="s">
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="79"/>
-      <c r="S5" s="79"/>
-      <c r="T5" s="79"/>
-      <c r="U5" s="79"/>
-      <c r="V5" s="80"/>
-      <c r="W5" s="78" t="s">
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="X5" s="79"/>
-      <c r="Y5" s="79"/>
-      <c r="Z5" s="79"/>
-      <c r="AA5" s="79"/>
-      <c r="AB5" s="80"/>
-      <c r="AC5" s="78" t="s">
+      <c r="X5" s="69"/>
+      <c r="Y5" s="69"/>
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="69"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="AD5" s="79"/>
-      <c r="AE5" s="79"/>
-      <c r="AF5" s="79"/>
-      <c r="AG5" s="79"/>
-      <c r="AH5" s="80"/>
-      <c r="AI5" s="78" t="s">
+      <c r="AD5" s="69"/>
+      <c r="AE5" s="69"/>
+      <c r="AF5" s="69"/>
+      <c r="AG5" s="69"/>
+      <c r="AH5" s="70"/>
+      <c r="AI5" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="AJ5" s="79"/>
-      <c r="AK5" s="79"/>
-      <c r="AL5" s="79"/>
-      <c r="AM5" s="79"/>
-      <c r="AN5" s="80"/>
-      <c r="AO5" s="78" t="s">
+      <c r="AJ5" s="69"/>
+      <c r="AK5" s="69"/>
+      <c r="AL5" s="69"/>
+      <c r="AM5" s="69"/>
+      <c r="AN5" s="70"/>
+      <c r="AO5" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="AP5" s="79"/>
-      <c r="AQ5" s="79"/>
-      <c r="AR5" s="79"/>
-      <c r="AS5" s="79"/>
-      <c r="AT5" s="80"/>
+      <c r="AP5" s="69"/>
+      <c r="AQ5" s="69"/>
+      <c r="AR5" s="69"/>
+      <c r="AS5" s="69"/>
+      <c r="AT5" s="70"/>
     </row>
     <row r="6" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="82"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="86"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="89"/>
       <c r="E6" s="10" t="s">
         <v>15</v>
       </c>
@@ -6972,10 +7082,10 @@
       <c r="AT7" s="7"/>
     </row>
     <row r="8" spans="1:46" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="87"/>
-      <c r="B8" s="87"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -7020,80 +7130,80 @@
       <c r="AT8" s="8"/>
     </row>
     <row r="9" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="83" t="s">
+      <c r="B9" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="78" t="s">
+      <c r="E9" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="79"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="78" t="s">
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="79"/>
-      <c r="M9" s="79"/>
-      <c r="N9" s="79"/>
-      <c r="O9" s="79"/>
-      <c r="P9" s="80"/>
-      <c r="Q9" s="78" t="s">
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="70"/>
+      <c r="Q9" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R9" s="79"/>
-      <c r="S9" s="79"/>
-      <c r="T9" s="79"/>
-      <c r="U9" s="79"/>
-      <c r="V9" s="80"/>
-      <c r="W9" s="78" t="s">
+      <c r="R9" s="69"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="X9" s="79"/>
-      <c r="Y9" s="79"/>
-      <c r="Z9" s="79"/>
-      <c r="AA9" s="79"/>
-      <c r="AB9" s="80"/>
-      <c r="AC9" s="78" t="s">
+      <c r="X9" s="69"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="70"/>
+      <c r="AC9" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="AD9" s="79"/>
-      <c r="AE9" s="79"/>
-      <c r="AF9" s="79"/>
-      <c r="AG9" s="79"/>
-      <c r="AH9" s="80"/>
-      <c r="AI9" s="78" t="s">
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="69"/>
+      <c r="AH9" s="70"/>
+      <c r="AI9" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="AJ9" s="79"/>
-      <c r="AK9" s="79"/>
-      <c r="AL9" s="79"/>
-      <c r="AM9" s="79"/>
-      <c r="AN9" s="80"/>
-      <c r="AO9" s="78" t="s">
+      <c r="AJ9" s="69"/>
+      <c r="AK9" s="69"/>
+      <c r="AL9" s="69"/>
+      <c r="AM9" s="69"/>
+      <c r="AN9" s="70"/>
+      <c r="AO9" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="AP9" s="79"/>
-      <c r="AQ9" s="79"/>
-      <c r="AR9" s="79"/>
-      <c r="AS9" s="79"/>
-      <c r="AT9" s="80"/>
+      <c r="AP9" s="69"/>
+      <c r="AQ9" s="69"/>
+      <c r="AR9" s="69"/>
+      <c r="AS9" s="69"/>
+      <c r="AT9" s="70"/>
     </row>
     <row r="10" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="87"/>
       <c r="E10" s="10" t="s">
         <v>15</v>
       </c>
@@ -7270,10 +7380,10 @@
       <c r="AT11" s="7"/>
     </row>
     <row r="12" spans="1:46" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="87"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -7350,14 +7460,14 @@
       <c r="A18" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="74"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="96"/>
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
@@ -7369,14 +7479,14 @@
       <c r="A19" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="77"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="98"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="99"/>
       <c r="K19" s="28"/>
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
@@ -7385,42 +7495,42 @@
       <c r="A20" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="77"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="99"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="77"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="99"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="93"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
@@ -7435,51 +7545,51 @@
       <c r="A24" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="70"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="91"/>
+      <c r="G24" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C4"/>
+    <mergeCell ref="D2:F4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="G2:J4"/>
+    <mergeCell ref="K9:P9"/>
+    <mergeCell ref="Q5:V5"/>
+    <mergeCell ref="Q9:V9"/>
+    <mergeCell ref="W5:AB5"/>
+    <mergeCell ref="W9:AB9"/>
+    <mergeCell ref="K5:P5"/>
     <mergeCell ref="AC5:AH5"/>
     <mergeCell ref="AC9:AH9"/>
     <mergeCell ref="AI5:AN5"/>
     <mergeCell ref="AI9:AN9"/>
     <mergeCell ref="AO5:AT5"/>
     <mergeCell ref="AO9:AT9"/>
-    <mergeCell ref="K9:P9"/>
-    <mergeCell ref="Q5:V5"/>
-    <mergeCell ref="Q9:V9"/>
-    <mergeCell ref="W5:AB5"/>
-    <mergeCell ref="W9:AB9"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C4"/>
-    <mergeCell ref="D2:F4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="G2:J4"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.23622047244094491" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="45" orientation="landscape" r:id="rId1"/>
@@ -7792,56 +7902,56 @@
       <c r="A22" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="74"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="95"/>
+      <c r="G22" s="96"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="77"/>
+      <c r="C23" s="98"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="99"/>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="77"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="98"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="99"/>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="75" t="s">
+      <c r="B25" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="77"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="99"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7851,11 +7961,11 @@
       <c r="B26" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="70"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="92"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7872,14 +7982,14 @@
       <c r="A28" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="70"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Ajuste status do processamento
</commit_message>
<xml_diff>
--- a/Modelo_PDO.xlsx
+++ b/Modelo_PDO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rogerio.piccoli\OneDrive\Documentos\GUAIBA\Python\ERG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70ac05f72bfee68d/Documentos/GUAIBA/Python/ERG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13254F7A-66E4-41EE-A861-21CCAE8D5F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{13254F7A-66E4-41EE-A861-21CCAE8D5F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D5F9767-DEB9-4D22-8F33-8458A6319E07}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conferência" sheetId="10" r:id="rId1"/>
@@ -1367,6 +1367,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1374,27 +1395,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1463,7 +1463,322 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="79">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2396,44 +2711,48 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1382" displayName="Tabela1382" ref="A10:F11" insertRow="1" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1382" displayName="Tabela1382" ref="A10:F11" insertRow="1" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A10:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DIAS ÚTEIS" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SABADOS " dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DIAS ÚTEIS2" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SABADOS 2" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DIAS ÚTEIS" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SABADOS " dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DIAS ÚTEIS2" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SABADOS 2" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela13493" displayName="Tabela13493" ref="A14:F15" insertRow="1" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela13493" displayName="Tabela13493" ref="A14:F15" insertRow="1" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <autoFilter ref="A14:F15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DIAS ÚTEIS" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SABADOS " dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DIAS ÚTEIS2" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="SABADOS 2" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DIAS ÚTEIS" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="SABADOS " dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DOMINGOS/FERIADOS" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DIAS ÚTEIS2" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="SABADOS 2" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DOMINGOS/FERIADOS2" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela94" displayName="Tabela94" ref="A4:D7" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela94" displayName="Tabela94" ref="A4:D7" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" tableBorderDxfId="60">
   <autoFilter ref="A4:D7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="####" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Total de Viagens Oficiais " dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Total de Viagens Extras" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Km's Totais" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="####" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Total de Viagens Oficiais " dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Total de Viagens Extras" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Km's Totais" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2731,9 +3050,7 @@
   </sheetPr>
   <dimension ref="A1:AK50"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2958,7 +3275,7 @@
       <c r="E4" s="48"/>
       <c r="F4" s="60"/>
       <c r="G4" s="49">
-        <f>D4+E4-F4</f>
+        <f>D4+E4+F4</f>
         <v>0</v>
       </c>
       <c r="H4" s="50"/>
@@ -2970,7 +3287,7 @@
       <c r="K4" s="48"/>
       <c r="L4" s="60"/>
       <c r="M4" s="49">
-        <f>J4+K4-L4</f>
+        <f>J4+K4+L4</f>
         <v>0</v>
       </c>
       <c r="N4" s="50"/>
@@ -2982,7 +3299,7 @@
       <c r="Q4" s="48"/>
       <c r="R4" s="60"/>
       <c r="S4" s="49">
-        <f>P4+Q4-R4</f>
+        <f>P4+Q4+R4</f>
         <v>0</v>
       </c>
       <c r="T4" s="50"/>
@@ -2994,7 +3311,7 @@
       <c r="W4" s="48"/>
       <c r="X4" s="60"/>
       <c r="Y4" s="49">
-        <f>V4+W4-X4</f>
+        <f>V4+W4+X4</f>
         <v>0</v>
       </c>
       <c r="Z4" s="50"/>
@@ -3006,7 +3323,7 @@
       <c r="AC4" s="48"/>
       <c r="AD4" s="60"/>
       <c r="AE4" s="49">
-        <f>AB4+AC4-AD4</f>
+        <f>AB4+AC4+AD4</f>
         <v>0</v>
       </c>
       <c r="AF4" s="50"/>
@@ -3018,7 +3335,7 @@
       <c r="AI4" s="48"/>
       <c r="AJ4" s="60"/>
       <c r="AK4" s="49">
-        <f>AH4+AI4-AJ4</f>
+        <f>AH4+AI4+AJ4</f>
         <v>0</v>
       </c>
     </row>
@@ -3033,7 +3350,7 @@
       <c r="E5" s="52"/>
       <c r="F5" s="61"/>
       <c r="G5" s="49">
-        <f t="shared" ref="G5:G49" si="1">D5+E5-F5</f>
+        <f t="shared" ref="G5:G49" si="1">D5+E5+F5</f>
         <v>0</v>
       </c>
       <c r="H5" s="53"/>
@@ -3045,7 +3362,7 @@
       <c r="K5" s="52"/>
       <c r="L5" s="61"/>
       <c r="M5" s="49">
-        <f t="shared" ref="M5:M49" si="3">J5+K5-L5</f>
+        <f t="shared" ref="M5:M49" si="3">J5+K5+L5</f>
         <v>0</v>
       </c>
       <c r="N5" s="53"/>
@@ -3057,7 +3374,7 @@
       <c r="Q5" s="52"/>
       <c r="R5" s="61"/>
       <c r="S5" s="49">
-        <f t="shared" ref="S5:S49" si="5">P5+Q5-R5</f>
+        <f t="shared" ref="S5:S49" si="5">P5+Q5+R5</f>
         <v>0</v>
       </c>
       <c r="T5" s="53"/>
@@ -3069,7 +3386,7 @@
       <c r="W5" s="52"/>
       <c r="X5" s="61"/>
       <c r="Y5" s="49">
-        <f t="shared" ref="Y5:Y49" si="7">V5+W5-X5</f>
+        <f t="shared" ref="Y5:Y49" si="7">V5+W5+X5</f>
         <v>0</v>
       </c>
       <c r="Z5" s="53"/>
@@ -3081,7 +3398,7 @@
       <c r="AC5" s="52"/>
       <c r="AD5" s="61"/>
       <c r="AE5" s="49">
-        <f t="shared" ref="AE5:AE49" si="9">AB5+AC5-AD5</f>
+        <f t="shared" ref="AE5:AE49" si="9">AB5+AC5+AD5</f>
         <v>0</v>
       </c>
       <c r="AF5" s="53"/>
@@ -3093,7 +3410,7 @@
       <c r="AI5" s="52"/>
       <c r="AJ5" s="61"/>
       <c r="AK5" s="49">
-        <f t="shared" ref="AK5:AK49" si="11">AH5+AI5-AJ5</f>
+        <f t="shared" ref="AK5:AK49" si="11">AH5+AI5+AJ5</f>
         <v>0</v>
       </c>
     </row>
@@ -6556,58 +6873,70 @@
     <mergeCell ref="T2:Y2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:F49">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G50 M4:M50 S4:S50 Y4:Y50 AE4:AE50 AK4:AK50">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:L49">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:R49">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:X49">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4:AD49">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH4:AJ49">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:E49">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:K49">
+    <cfRule type="cellIs" dxfId="4" priority="13" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V4:W49">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:Q49">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH4:AI49">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThan">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB4:AC49">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6621,8 +6950,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:AT18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6732,80 +7061,80 @@
       <c r="J4" s="98"/>
     </row>
     <row r="5" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="82" t="s">
+      <c r="B5" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="77" t="s">
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="79"/>
-      <c r="Q5" s="77" t="s">
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
-      <c r="U5" s="78"/>
-      <c r="V5" s="79"/>
-      <c r="W5" s="77" t="s">
+      <c r="R5" s="85"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="X5" s="78"/>
-      <c r="Y5" s="78"/>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="78"/>
-      <c r="AB5" s="79"/>
-      <c r="AC5" s="77" t="s">
+      <c r="X5" s="85"/>
+      <c r="Y5" s="85"/>
+      <c r="Z5" s="85"/>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="86"/>
+      <c r="AC5" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="AD5" s="78"/>
-      <c r="AE5" s="78"/>
-      <c r="AF5" s="78"/>
-      <c r="AG5" s="78"/>
-      <c r="AH5" s="79"/>
-      <c r="AI5" s="77" t="s">
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="85"/>
+      <c r="AG5" s="85"/>
+      <c r="AH5" s="86"/>
+      <c r="AI5" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="AJ5" s="78"/>
-      <c r="AK5" s="78"/>
-      <c r="AL5" s="78"/>
-      <c r="AM5" s="78"/>
-      <c r="AN5" s="79"/>
-      <c r="AO5" s="77" t="s">
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="85"/>
+      <c r="AN5" s="86"/>
+      <c r="AO5" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="AP5" s="78"/>
-      <c r="AQ5" s="78"/>
-      <c r="AR5" s="78"/>
-      <c r="AS5" s="78"/>
-      <c r="AT5" s="79"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
     </row>
     <row r="6" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="81"/>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="85"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="9" t="s">
         <v>15</v>
       </c>
@@ -6982,10 +7311,10 @@
       <c r="AT7" s="6"/>
     </row>
     <row r="8" spans="1:46" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
+      <c r="A8" s="77"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -7184,7 +7513,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>